<commit_message>
Finished W02, implementing W03
</commit_message>
<xml_diff>
--- a/testcase/OpenERP_TCs for automation training course.xlsx
+++ b/testcase/OpenERP_TCs for automation training course.xlsx
@@ -15106,10 +15106,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="11" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>